<commit_message>
Delete proprietary CIC + FPGA code optimization
</commit_message>
<xml_diff>
--- a/Scheme/Decimation.xlsx
+++ b/Scheme/Decimation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Частота кварцевого генератора,гц</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>*все коэффициенты должны быть степенью двойки (2,4,8,16,32,…)</t>
+  </si>
+  <si>
+    <t>Полученная частота дискретизации CIC коспенсатора</t>
   </si>
 </sst>
 </file>
@@ -111,12 +114,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +441,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="3">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -444,7 +450,7 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -490,41 +496,54 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4">
+        <f>C7/C9</f>
+        <v>95969.289827255285</v>
+      </c>
+      <c r="D10">
+        <f>D7/D9</f>
+        <v>97656.25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <f>C7/C9/C8</f>
         <v>47984.644913627642</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D11" s="4">
         <f>D7/D9/D8</f>
         <v>48828.125</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4">
-        <f>C10-C3</f>
-        <v>-15.355086372357619</v>
-      </c>
-      <c r="D11" s="4">
-        <f>D10-C3</f>
-        <v>828.125</v>
-      </c>
-    </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <f>C11-C3</f>
+        <v>-15.355086372357619</v>
+      </c>
+      <c r="D12" s="4">
+        <f>D11-C3</f>
+        <v>828.125</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C13" s="4">
         <f>C7*C4/C9</f>
-        <v>2303262.9558541267</v>
-      </c>
-      <c r="D12" s="4">
+        <v>3262955.8541266792</v>
+      </c>
+      <c r="D13" s="4">
         <f>D7*C4/D9</f>
-        <v>2343750</v>
+        <v>3320312.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch to 49.152 Clock Generator
</commit_message>
<xml_diff>
--- a/Scheme/Decimation.xlsx
+++ b/Scheme/Decimation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Частота кварцевого генератора,гц</t>
   </si>
@@ -50,19 +50,22 @@
     <t>Коэффициент децимации/интерполяции CIC фильтра</t>
   </si>
   <si>
-    <t>Частота для CIC компенсатора RX/TX,гц</t>
-  </si>
-  <si>
-    <t>Clock rate при расчёте CIC компенсатора</t>
-  </si>
-  <si>
-    <t>Практика</t>
-  </si>
-  <si>
     <t>*все коэффициенты должны быть степенью двойки (2,4,8,16,32,…)</t>
   </si>
   <si>
     <t>Полученная частота дискретизации CIC коспенсатора</t>
+  </si>
+  <si>
+    <t>Clock rate при расчёте CIC компенсатора RX</t>
+  </si>
+  <si>
+    <t>Clock rate при расчёте CIC компенсатора TX</t>
+  </si>
+  <si>
+    <t>Частота для CIC компенсатора RX,гц</t>
+  </si>
+  <si>
+    <t>Частота для I2S шины</t>
   </si>
 </sst>
 </file>
@@ -114,15 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -403,30 +403,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="58.140625" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>50000000</v>
+        <v>49152000</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -434,116 +432,111 @@
         <v>48000</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f>C2</f>
+        <v>49152000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f>MROUND(C8/C9/C3,1)</f>
+        <v>512</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
-        <v>34</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <f>C2</f>
-        <v>50000000</v>
-      </c>
-      <c r="D7">
-        <f>C7</f>
-        <v>50000000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <f>C8</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <f>MROUND(C7/C8/C3,1)</f>
-        <v>521</v>
-      </c>
-      <c r="D9">
-        <v>512</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C11" s="4">
+        <f>C8/C10</f>
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4">
+        <f>C8/C10/C9</f>
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4">
+        <f>C12-C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4">
-        <f>C7/C9</f>
-        <v>95969.289827255285</v>
-      </c>
-      <c r="D10">
-        <f>D7/D9</f>
-        <v>97656.25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="4">
-        <f>C7/C9/C8</f>
-        <v>47984.644913627642</v>
-      </c>
-      <c r="D11" s="4">
-        <f>D7/D9/D8</f>
-        <v>48828.125</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="4">
-        <f>C11-C3</f>
-        <v>-15.355086372357619</v>
-      </c>
-      <c r="D12" s="4">
-        <f>D11-C3</f>
-        <v>828.125</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="4">
-        <f>C7*C4/C9</f>
-        <v>3262955.8541266792</v>
-      </c>
-      <c r="D13" s="4">
-        <f>D7*C4/D9</f>
-        <v>3320312.5</v>
+      <c r="C14" s="4">
+        <f>C8*C4/C10</f>
+        <v>1536000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4">
+        <f>C8*C5/C10</f>
+        <v>1344000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <f>C12*256</f>
+        <v>12288000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>